<commit_message>
Added England and Wales analysis.
</commit_message>
<xml_diff>
--- a/ONSDeathStats.xlsx
+++ b/ONSDeathStats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\source\repos\Covid19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CE47AC1-7C2D-4886-97C8-4D28A5DEC4D5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6101FB6-B7DB-4B9F-9C49-C2D95205E730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B79DB374-28FF-483D-B0D3-E7518FBA4BC4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{B79DB374-28FF-483D-B0D3-E7518FBA4BC4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Nottinghamshire" sheetId="1" r:id="rId1"/>
+    <sheet name="England and Wales" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
   <si>
     <t>E10000024</t>
   </si>
@@ -349,16 +350,89 @@
   <si>
     <t>https://www.ons.gov.uk/peoplepopulationandcommunity/birthsdeathsandmarriages/deaths/datasets/monthlyfiguresondeathsregisteredbyareaofusualresidence</t>
   </si>
+  <si>
+    <t>K04000001</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>ENGLAND AND WALES 2020</t>
+  </si>
+  <si>
+    <t>ENGLAND AND WALES 2019</t>
+  </si>
+  <si>
+    <t>ENGLAND AND WALES 2018</t>
+  </si>
+  <si>
+    <t>ENGLAND AND WALES 2017</t>
+  </si>
+  <si>
+    <t>ENGLAND AND WALES 2016</t>
+  </si>
+  <si>
+    <t>ENGLAND AND WALES 2015</t>
+  </si>
+  <si>
+    <t>5 Year Mean Excluding 2020</t>
+  </si>
+  <si>
+    <t>2020 Excess over 5 Year Mean</t>
+  </si>
+  <si>
+    <t>Number of Std Deviations</t>
+  </si>
+  <si>
+    <t>5 Year Std Dev Excluding 2020</t>
+  </si>
+  <si>
+    <t>Total to Sep</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="General_)"/>
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="General_)"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,11 +464,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Helv"/>
     </font>
     <font>
@@ -406,6 +475,33 @@
     <font>
       <vertAlign val="superscript"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -438,16 +534,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -456,14 +552,16 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7"/>
@@ -474,7 +572,7 @@
     <xf numFmtId="17" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="17" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -485,7 +583,7 @@
     <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="17" fontId="8" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="7" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7"/>
@@ -501,10 +599,49 @@
     <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="7" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="16">
     <cellStyle name="Comma 2" xfId="2" xr:uid="{2DF0F7EA-ABE1-49E7-9343-B35E15EBCEE0}"/>
+    <cellStyle name="Comma 2 2" xfId="14" xr:uid="{449E8343-4D4D-41CE-AF14-2E8B75ACFE89}"/>
     <cellStyle name="Comma 3" xfId="3" xr:uid="{313870A5-27BF-4B8B-BDD9-5577E35C0A35}"/>
+    <cellStyle name="Comma 3 2" xfId="15" xr:uid="{D24DFE83-4438-4A16-BC83-B27DBD137533}"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="5" xr:uid="{73E8154D-BE47-41FE-B242-48C0CB67A5A2}"/>
     <cellStyle name="Hyperlink 2 2" xfId="6" xr:uid="{81302E0B-1E6D-4CB0-9F60-315B57E97192}"/>
@@ -830,9 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7680C988-E5D9-431B-81FB-B9CE46BEA452}">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2079,4 +2214,579 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589DD6B3-9915-4FCA-8F45-2E3BAB680481}">
+  <dimension ref="A1:P15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="11" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="43" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="43"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C3" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="J3" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="L3" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="37">
+        <v>56597</v>
+      </c>
+      <c r="D4" s="37">
+        <v>43555</v>
+      </c>
+      <c r="E4" s="37">
+        <v>49641</v>
+      </c>
+      <c r="F4" s="29">
+        <v>88049</v>
+      </c>
+      <c r="G4" s="29">
+        <v>52315</v>
+      </c>
+      <c r="H4" s="37">
+        <v>42577</v>
+      </c>
+      <c r="I4" s="37">
+        <v>40731</v>
+      </c>
+      <c r="J4" s="37">
+        <v>37129</v>
+      </c>
+      <c r="K4" s="37">
+        <v>42432</v>
+      </c>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="P4" s="26">
+        <f>SUM(C4:K4)</f>
+        <v>453026</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="37">
+        <v>53774</v>
+      </c>
+      <c r="D5" s="37">
+        <v>45695</v>
+      </c>
+      <c r="E5" s="37">
+        <v>43817</v>
+      </c>
+      <c r="F5" s="37">
+        <v>44005</v>
+      </c>
+      <c r="G5" s="37">
+        <v>44292</v>
+      </c>
+      <c r="H5" s="37">
+        <v>38511</v>
+      </c>
+      <c r="I5" s="37">
+        <v>42192</v>
+      </c>
+      <c r="J5" s="37">
+        <v>38721</v>
+      </c>
+      <c r="K5" s="37">
+        <v>39915</v>
+      </c>
+      <c r="L5" s="37">
+        <v>46131</v>
+      </c>
+      <c r="M5" s="37">
+        <v>45124</v>
+      </c>
+      <c r="N5" s="37">
+        <v>47376</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:P9" si="0">SUM(C5:K5)</f>
+        <v>390922</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="27">
+        <v>64020</v>
+      </c>
+      <c r="D6" s="27">
+        <v>49087</v>
+      </c>
+      <c r="E6" s="27">
+        <v>51131</v>
+      </c>
+      <c r="F6" s="27">
+        <v>46383</v>
+      </c>
+      <c r="G6" s="27">
+        <v>42685</v>
+      </c>
+      <c r="H6" s="27">
+        <v>39679</v>
+      </c>
+      <c r="I6" s="27">
+        <v>40621</v>
+      </c>
+      <c r="J6" s="27">
+        <v>40071</v>
+      </c>
+      <c r="K6" s="27">
+        <v>37013</v>
+      </c>
+      <c r="L6" s="27">
+        <v>44311</v>
+      </c>
+      <c r="M6" s="27">
+        <v>43834</v>
+      </c>
+      <c r="N6" s="27">
+        <v>41430</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>410690</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="36">
+        <v>57266</v>
+      </c>
+      <c r="D7" s="36">
+        <v>47695</v>
+      </c>
+      <c r="E7" s="36">
+        <v>48577</v>
+      </c>
+      <c r="F7" s="36">
+        <v>39024</v>
+      </c>
+      <c r="G7" s="36">
+        <v>44183</v>
+      </c>
+      <c r="H7" s="36">
+        <v>42074</v>
+      </c>
+      <c r="I7" s="36">
+        <v>38314</v>
+      </c>
+      <c r="J7" s="36">
+        <v>40963</v>
+      </c>
+      <c r="K7" s="36">
+        <v>40002</v>
+      </c>
+      <c r="L7" s="36">
+        <v>43504</v>
+      </c>
+      <c r="M7" s="36">
+        <v>45476</v>
+      </c>
+      <c r="N7" s="36">
+        <v>45052</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>398098</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="36">
+        <v>47351</v>
+      </c>
+      <c r="D8" s="36">
+        <v>45922</v>
+      </c>
+      <c r="E8" s="36">
+        <v>48562</v>
+      </c>
+      <c r="F8" s="36">
+        <v>46755</v>
+      </c>
+      <c r="G8" s="36">
+        <v>41291</v>
+      </c>
+      <c r="H8" s="36">
+        <v>41921</v>
+      </c>
+      <c r="I8" s="36">
+        <v>38882</v>
+      </c>
+      <c r="J8" s="36">
+        <v>40676</v>
+      </c>
+      <c r="K8" s="36">
+        <v>40250</v>
+      </c>
+      <c r="L8" s="36">
+        <v>40360</v>
+      </c>
+      <c r="M8" s="36">
+        <v>46418</v>
+      </c>
+      <c r="N8" s="36">
+        <v>45469</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>391610</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="36">
+        <v>60779</v>
+      </c>
+      <c r="D9" s="36">
+        <v>46634</v>
+      </c>
+      <c r="E9" s="36">
+        <v>47820</v>
+      </c>
+      <c r="F9" s="36">
+        <v>45077</v>
+      </c>
+      <c r="G9" s="36">
+        <v>39250</v>
+      </c>
+      <c r="H9" s="36">
+        <v>41992</v>
+      </c>
+      <c r="I9" s="36">
+        <v>40400</v>
+      </c>
+      <c r="J9" s="36">
+        <v>36096</v>
+      </c>
+      <c r="K9" s="36">
+        <v>41491</v>
+      </c>
+      <c r="L9" s="36">
+        <v>42125</v>
+      </c>
+      <c r="M9" s="36">
+        <v>41431</v>
+      </c>
+      <c r="N9" s="36">
+        <v>45412</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>399539</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="45"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="45"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="45">
+        <f>AVERAGE(C5:C9)</f>
+        <v>56638</v>
+      </c>
+      <c r="D11" s="45">
+        <f t="shared" ref="D11:N11" si="1">AVERAGE(D5:D9)</f>
+        <v>47006.6</v>
+      </c>
+      <c r="E11" s="45">
+        <f t="shared" si="1"/>
+        <v>47981.4</v>
+      </c>
+      <c r="F11" s="45">
+        <f t="shared" si="1"/>
+        <v>44248.800000000003</v>
+      </c>
+      <c r="G11" s="45">
+        <f t="shared" si="1"/>
+        <v>42340.2</v>
+      </c>
+      <c r="H11" s="45">
+        <f t="shared" si="1"/>
+        <v>40835.4</v>
+      </c>
+      <c r="I11" s="45">
+        <f t="shared" si="1"/>
+        <v>40081.800000000003</v>
+      </c>
+      <c r="J11" s="45">
+        <f t="shared" si="1"/>
+        <v>39305.4</v>
+      </c>
+      <c r="K11" s="45">
+        <f t="shared" si="1"/>
+        <v>39734.199999999997</v>
+      </c>
+      <c r="L11" s="45">
+        <f t="shared" si="1"/>
+        <v>43286.2</v>
+      </c>
+      <c r="M11" s="45">
+        <f t="shared" si="1"/>
+        <v>44456.6</v>
+      </c>
+      <c r="N11" s="45">
+        <f t="shared" si="1"/>
+        <v>44947.8</v>
+      </c>
+      <c r="P11" s="45">
+        <f t="shared" ref="P11" si="2">AVERAGE(P5:P9)</f>
+        <v>398171.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="45">
+        <f>_xlfn.STDEV.S(C5:C9)</f>
+        <v>6451.4931217509638</v>
+      </c>
+      <c r="D12" s="45">
+        <f t="shared" ref="D12:N12" si="3">_xlfn.STDEV.S(D5:D9)</f>
+        <v>1399.7715170698395</v>
+      </c>
+      <c r="E12" s="45">
+        <f t="shared" si="3"/>
+        <v>2644.8106359435264</v>
+      </c>
+      <c r="F12" s="45">
+        <f t="shared" si="3"/>
+        <v>3117.6809009261997</v>
+      </c>
+      <c r="G12" s="45">
+        <f t="shared" si="3"/>
+        <v>2119.8159589926668</v>
+      </c>
+      <c r="H12" s="45">
+        <f t="shared" si="3"/>
+        <v>1642.4430888161696</v>
+      </c>
+      <c r="I12" s="45">
+        <f t="shared" si="3"/>
+        <v>1533.7510228195449</v>
+      </c>
+      <c r="J12" s="45">
+        <f t="shared" si="3"/>
+        <v>1990.8601909727363</v>
+      </c>
+      <c r="K12" s="45">
+        <f t="shared" si="3"/>
+        <v>1647.8570022911576</v>
+      </c>
+      <c r="L12" s="45">
+        <f t="shared" si="3"/>
+        <v>2185.267191901256</v>
+      </c>
+      <c r="M12" s="45">
+        <f t="shared" si="3"/>
+        <v>1928.3137192894731</v>
+      </c>
+      <c r="N12" s="45">
+        <f t="shared" si="3"/>
+        <v>2166.1637057249391</v>
+      </c>
+      <c r="P12" s="45">
+        <f t="shared" ref="P12" si="4">_xlfn.STDEV.S(P5:P9)</f>
+        <v>7971.7757243916485</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="6">
+        <f>C4-C11</f>
+        <v>-41</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" ref="D14:K14" si="5">D4-D11</f>
+        <v>-3451.5999999999985</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="5"/>
+        <v>1659.5999999999985</v>
+      </c>
+      <c r="F14" s="30">
+        <f t="shared" si="5"/>
+        <v>43800.2</v>
+      </c>
+      <c r="G14" s="30">
+        <f t="shared" si="5"/>
+        <v>9974.8000000000029</v>
+      </c>
+      <c r="H14" s="6">
+        <f t="shared" si="5"/>
+        <v>1741.5999999999985</v>
+      </c>
+      <c r="I14" s="6">
+        <f t="shared" si="5"/>
+        <v>649.19999999999709</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="5"/>
+        <v>-2176.4000000000015</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="5"/>
+        <v>2697.8000000000029</v>
+      </c>
+      <c r="P14" s="30">
+        <f t="shared" ref="P14" si="6">P4-P11</f>
+        <v>54854.200000000012</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15">
+        <f>C14/C12</f>
+        <v>-6.3551179899378734E-3</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:K15" si="7">D14/D12</f>
+        <v>-2.4658310002087189</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="7"/>
+        <v>0.62749293936045536</v>
+      </c>
+      <c r="F15" s="26">
+        <f t="shared" si="7"/>
+        <v>14.04896825296901</v>
+      </c>
+      <c r="G15" s="26">
+        <f t="shared" si="7"/>
+        <v>4.7055028327742248</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="7"/>
+        <v>1.0603715963487652</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="7"/>
+        <v>0.42327600134639282</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="7"/>
+        <v>-1.0931958004226354</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="7"/>
+        <v>1.6371566199306244</v>
+      </c>
+      <c r="P15" s="26">
+        <f t="shared" ref="P15" si="8">P14/P12</f>
+        <v>6.8810515870585549</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{02A692E6-3128-4B43-9670-44C7F1AAEA63}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>